<commit_message>
added Insert new CHEMProduct regression test
</commit_message>
<xml_diff>
--- a/src/RegressionTests/Katalon/inputFiles/ht_dna_generateOrder4Katalon.xlsx
+++ b/src/RegressionTests/Katalon/inputFiles/ht_dna_generateOrder4Katalon.xlsx
@@ -866,276 +866,6 @@
     <t>Alternate Name</t>
   </si>
   <si>
-    <t>TEST0000013</t>
-  </si>
-  <si>
-    <t>TEST0000026</t>
-  </si>
-  <si>
-    <t>TEST0000037</t>
-  </si>
-  <si>
-    <t>TEST0001397</t>
-  </si>
-  <si>
-    <t>TEST0001463</t>
-  </si>
-  <si>
-    <t>TEST0005460</t>
-  </si>
-  <si>
-    <t>TEST0005476</t>
-  </si>
-  <si>
-    <t>TEST0005477</t>
-  </si>
-  <si>
-    <t>TEST0005478</t>
-  </si>
-  <si>
-    <t>TEST0005479</t>
-  </si>
-  <si>
-    <t>TEST0005480</t>
-  </si>
-  <si>
-    <t>TEST0005481</t>
-  </si>
-  <si>
-    <t>TEST0005482</t>
-  </si>
-  <si>
-    <t>TEST0005483</t>
-  </si>
-  <si>
-    <t>TEST0005484</t>
-  </si>
-  <si>
-    <t>TEST0005485</t>
-  </si>
-  <si>
-    <t>TEST0005486</t>
-  </si>
-  <si>
-    <t>TEST0005487</t>
-  </si>
-  <si>
-    <t>TEST0005488</t>
-  </si>
-  <si>
-    <t>TEST0005489</t>
-  </si>
-  <si>
-    <t>TEST0005490</t>
-  </si>
-  <si>
-    <t>TEST0005491</t>
-  </si>
-  <si>
-    <t>TEST0005492</t>
-  </si>
-  <si>
-    <t>TEST0005493</t>
-  </si>
-  <si>
-    <t>TEST0005494</t>
-  </si>
-  <si>
-    <t>TEST0005495</t>
-  </si>
-  <si>
-    <t>TEST0005496</t>
-  </si>
-  <si>
-    <t>TEST0005497</t>
-  </si>
-  <si>
-    <t>TEST0005498</t>
-  </si>
-  <si>
-    <t>TEST0005499</t>
-  </si>
-  <si>
-    <t>TEST0005500</t>
-  </si>
-  <si>
-    <t>TEST0005501</t>
-  </si>
-  <si>
-    <t>TEST0005502</t>
-  </si>
-  <si>
-    <t>TEST0005503</t>
-  </si>
-  <si>
-    <t>TEST0005504</t>
-  </si>
-  <si>
-    <t>TEST0005505</t>
-  </si>
-  <si>
-    <t>TEST0005506</t>
-  </si>
-  <si>
-    <t>TEST0005507</t>
-  </si>
-  <si>
-    <t>TEST0005508</t>
-  </si>
-  <si>
-    <t>TEST0005509</t>
-  </si>
-  <si>
-    <t>TEST0005510</t>
-  </si>
-  <si>
-    <t>TEST0005511</t>
-  </si>
-  <si>
-    <t>TEST0005512</t>
-  </si>
-  <si>
-    <t>TEST0005513</t>
-  </si>
-  <si>
-    <t>TEST0005514</t>
-  </si>
-  <si>
-    <t>TEST0005515</t>
-  </si>
-  <si>
-    <t>TEST0005516</t>
-  </si>
-  <si>
-    <t>TEST0005517</t>
-  </si>
-  <si>
-    <t>TEST0005518</t>
-  </si>
-  <si>
-    <t>TEST0005519</t>
-  </si>
-  <si>
-    <t>TEST0005520</t>
-  </si>
-  <si>
-    <t>TEST0005521</t>
-  </si>
-  <si>
-    <t>TEST0005522</t>
-  </si>
-  <si>
-    <t>TEST0005523</t>
-  </si>
-  <si>
-    <t>TEST0005524</t>
-  </si>
-  <si>
-    <t>TEST0005525</t>
-  </si>
-  <si>
-    <t>TEST0005526</t>
-  </si>
-  <si>
-    <t>TEST0005527</t>
-  </si>
-  <si>
-    <t>TEST0005528</t>
-  </si>
-  <si>
-    <t>TEST0005529</t>
-  </si>
-  <si>
-    <t>TEST0005530</t>
-  </si>
-  <si>
-    <t>TEST0005531</t>
-  </si>
-  <si>
-    <t>TEST0005532</t>
-  </si>
-  <si>
-    <t>TEST0005533</t>
-  </si>
-  <si>
-    <t>TEST0005534</t>
-  </si>
-  <si>
-    <t>TEST0005535</t>
-  </si>
-  <si>
-    <t>TEST0005536</t>
-  </si>
-  <si>
-    <t>TEST0005537</t>
-  </si>
-  <si>
-    <t>TEST0005538</t>
-  </si>
-  <si>
-    <t>TEST0005539</t>
-  </si>
-  <si>
-    <t>TEST0005540</t>
-  </si>
-  <si>
-    <t>TEST0005541</t>
-  </si>
-  <si>
-    <t>TEST0005542</t>
-  </si>
-  <si>
-    <t>TEST0005543</t>
-  </si>
-  <si>
-    <t>TEST0005544</t>
-  </si>
-  <si>
-    <t>TEST0005545</t>
-  </si>
-  <si>
-    <t>TEST0005546</t>
-  </si>
-  <si>
-    <t>TEST0005547</t>
-  </si>
-  <si>
-    <t>TEST0005548</t>
-  </si>
-  <si>
-    <t>TEST0005549</t>
-  </si>
-  <si>
-    <t>TEST0005550</t>
-  </si>
-  <si>
-    <t>TEST0005551</t>
-  </si>
-  <si>
-    <t>TEST0005552</t>
-  </si>
-  <si>
-    <t>TEST0005553</t>
-  </si>
-  <si>
-    <t>TEST0005554</t>
-  </si>
-  <si>
-    <t>TEST0005555</t>
-  </si>
-  <si>
-    <t>TEST0005556</t>
-  </si>
-  <si>
-    <t>TEST0005557</t>
-  </si>
-  <si>
-    <t>TEST0005645</t>
-  </si>
-  <si>
-    <t>TEST0005647</t>
-  </si>
-  <si>
     <t>urn:lsid:fhcrc.org:Sample.9.Construct:TEST0000013</t>
   </si>
   <si>
@@ -1404,6 +1134,276 @@
   </si>
   <si>
     <t>urn:lsid:fhcrc.org:Sample.9.Construct:TEST0005647</t>
+  </si>
+  <si>
+    <t>TST0000013</t>
+  </si>
+  <si>
+    <t>TST0000026</t>
+  </si>
+  <si>
+    <t>TST0000037</t>
+  </si>
+  <si>
+    <t>TST0001397</t>
+  </si>
+  <si>
+    <t>TST0001463</t>
+  </si>
+  <si>
+    <t>TST0005460</t>
+  </si>
+  <si>
+    <t>TST0005476</t>
+  </si>
+  <si>
+    <t>TST0005477</t>
+  </si>
+  <si>
+    <t>TST0005478</t>
+  </si>
+  <si>
+    <t>TST0005479</t>
+  </si>
+  <si>
+    <t>TST0005480</t>
+  </si>
+  <si>
+    <t>TST0005481</t>
+  </si>
+  <si>
+    <t>TST0005482</t>
+  </si>
+  <si>
+    <t>TST0005483</t>
+  </si>
+  <si>
+    <t>TST0005484</t>
+  </si>
+  <si>
+    <t>TST0005485</t>
+  </si>
+  <si>
+    <t>TST0005486</t>
+  </si>
+  <si>
+    <t>TST0005487</t>
+  </si>
+  <si>
+    <t>TST0005488</t>
+  </si>
+  <si>
+    <t>TST0005489</t>
+  </si>
+  <si>
+    <t>TST0005490</t>
+  </si>
+  <si>
+    <t>TST0005491</t>
+  </si>
+  <si>
+    <t>TST0005492</t>
+  </si>
+  <si>
+    <t>TST0005493</t>
+  </si>
+  <si>
+    <t>TST0005494</t>
+  </si>
+  <si>
+    <t>TST0005495</t>
+  </si>
+  <si>
+    <t>TST0005496</t>
+  </si>
+  <si>
+    <t>TST0005497</t>
+  </si>
+  <si>
+    <t>TST0005498</t>
+  </si>
+  <si>
+    <t>TST0005499</t>
+  </si>
+  <si>
+    <t>TST0005500</t>
+  </si>
+  <si>
+    <t>TST0005501</t>
+  </si>
+  <si>
+    <t>TST0005502</t>
+  </si>
+  <si>
+    <t>TST0005503</t>
+  </si>
+  <si>
+    <t>TST0005504</t>
+  </si>
+  <si>
+    <t>TST0005505</t>
+  </si>
+  <si>
+    <t>TST0005506</t>
+  </si>
+  <si>
+    <t>TST0005507</t>
+  </si>
+  <si>
+    <t>TST0005508</t>
+  </si>
+  <si>
+    <t>TST0005509</t>
+  </si>
+  <si>
+    <t>TST0005510</t>
+  </si>
+  <si>
+    <t>TST0005511</t>
+  </si>
+  <si>
+    <t>TST0005512</t>
+  </si>
+  <si>
+    <t>TST0005513</t>
+  </si>
+  <si>
+    <t>TST0005514</t>
+  </si>
+  <si>
+    <t>TST0005515</t>
+  </si>
+  <si>
+    <t>TST0005516</t>
+  </si>
+  <si>
+    <t>TST0005517</t>
+  </si>
+  <si>
+    <t>TST0005518</t>
+  </si>
+  <si>
+    <t>TST0005519</t>
+  </si>
+  <si>
+    <t>TST0005520</t>
+  </si>
+  <si>
+    <t>TST0005521</t>
+  </si>
+  <si>
+    <t>TST0005522</t>
+  </si>
+  <si>
+    <t>TST0005523</t>
+  </si>
+  <si>
+    <t>TST0005524</t>
+  </si>
+  <si>
+    <t>TST0005525</t>
+  </si>
+  <si>
+    <t>TST0005526</t>
+  </si>
+  <si>
+    <t>TST0005527</t>
+  </si>
+  <si>
+    <t>TST0005528</t>
+  </si>
+  <si>
+    <t>TST0005529</t>
+  </si>
+  <si>
+    <t>TST0005530</t>
+  </si>
+  <si>
+    <t>TST0005531</t>
+  </si>
+  <si>
+    <t>TST0005532</t>
+  </si>
+  <si>
+    <t>TST0005533</t>
+  </si>
+  <si>
+    <t>TST0005534</t>
+  </si>
+  <si>
+    <t>TST0005535</t>
+  </si>
+  <si>
+    <t>TST0005536</t>
+  </si>
+  <si>
+    <t>TST0005537</t>
+  </si>
+  <si>
+    <t>TST0005538</t>
+  </si>
+  <si>
+    <t>TST0005539</t>
+  </si>
+  <si>
+    <t>TST0005540</t>
+  </si>
+  <si>
+    <t>TST0005541</t>
+  </si>
+  <si>
+    <t>TST0005542</t>
+  </si>
+  <si>
+    <t>TST0005543</t>
+  </si>
+  <si>
+    <t>TST0005544</t>
+  </si>
+  <si>
+    <t>TST0005545</t>
+  </si>
+  <si>
+    <t>TST0005546</t>
+  </si>
+  <si>
+    <t>TST0005547</t>
+  </si>
+  <si>
+    <t>TST0005548</t>
+  </si>
+  <si>
+    <t>TST0005549</t>
+  </si>
+  <si>
+    <t>TST0005550</t>
+  </si>
+  <si>
+    <t>TST0005551</t>
+  </si>
+  <si>
+    <t>TST0005552</t>
+  </si>
+  <si>
+    <t>TST0005553</t>
+  </si>
+  <si>
+    <t>TST0005554</t>
+  </si>
+  <si>
+    <t>TST0005555</t>
+  </si>
+  <si>
+    <t>TST0005556</t>
+  </si>
+  <si>
+    <t>TST0005557</t>
+  </si>
+  <si>
+    <t>TST0005645</t>
+  </si>
+  <si>
+    <t>TST0005647</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
         <v>280</v>
       </c>
-      <c r="B2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>370</v>
-      </c>
-      <c r="D2" t="s">
-        <v>280</v>
       </c>
       <c r="E2" t="s">
         <v>187</v>
@@ -1799,16 +1799,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
         <v>281</v>
       </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>371</v>
-      </c>
-      <c r="D3" t="s">
-        <v>281</v>
       </c>
       <c r="E3" t="s">
         <v>188</v>
@@ -1828,16 +1828,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
         <v>282</v>
       </c>
-      <c r="B4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>372</v>
-      </c>
-      <c r="D4" t="s">
-        <v>282</v>
       </c>
       <c r="E4" t="s">
         <v>189</v>
@@ -1857,16 +1857,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
         <v>283</v>
       </c>
-      <c r="B5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>373</v>
-      </c>
-      <c r="D5" t="s">
-        <v>283</v>
       </c>
       <c r="E5" t="s">
         <v>190</v>
@@ -1886,16 +1886,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>374</v>
+      </c>
+      <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" t="s">
         <v>284</v>
       </c>
-      <c r="B6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>374</v>
-      </c>
-      <c r="D6" t="s">
-        <v>284</v>
       </c>
       <c r="E6" t="s">
         <v>191</v>
@@ -1915,16 +1915,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" t="s">
         <v>285</v>
       </c>
-      <c r="B7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>375</v>
-      </c>
-      <c r="D7" t="s">
-        <v>285</v>
       </c>
       <c r="E7" t="s">
         <v>192</v>
@@ -1944,16 +1944,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" t="s">
         <v>286</v>
       </c>
-      <c r="B8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>376</v>
-      </c>
-      <c r="D8" t="s">
-        <v>286</v>
       </c>
       <c r="E8" t="s">
         <v>193</v>
@@ -1973,16 +1973,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" t="s">
         <v>287</v>
       </c>
-      <c r="B9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>377</v>
-      </c>
-      <c r="D9" t="s">
-        <v>287</v>
       </c>
       <c r="E9" t="s">
         <v>194</v>
@@ -2002,16 +2002,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>378</v>
+      </c>
+      <c r="B10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" t="s">
         <v>288</v>
       </c>
-      <c r="B10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>378</v>
-      </c>
-      <c r="D10" t="s">
-        <v>288</v>
       </c>
       <c r="E10" t="s">
         <v>195</v>
@@ -2031,16 +2031,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" t="s">
         <v>289</v>
       </c>
-      <c r="B11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>379</v>
-      </c>
-      <c r="D11" t="s">
-        <v>289</v>
       </c>
       <c r="E11" t="s">
         <v>196</v>
@@ -2060,16 +2060,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" t="s">
         <v>290</v>
       </c>
-      <c r="B12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>380</v>
-      </c>
-      <c r="D12" t="s">
-        <v>290</v>
       </c>
       <c r="E12" t="s">
         <v>197</v>
@@ -2089,16 +2089,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>381</v>
+      </c>
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" t="s">
         <v>291</v>
       </c>
-      <c r="B13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>381</v>
-      </c>
-      <c r="D13" t="s">
-        <v>291</v>
       </c>
       <c r="E13" t="s">
         <v>198</v>
@@ -2118,16 +2118,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" t="s">
         <v>292</v>
       </c>
-      <c r="B14" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>382</v>
-      </c>
-      <c r="D14" t="s">
-        <v>292</v>
       </c>
       <c r="E14" t="s">
         <v>199</v>
@@ -2147,16 +2147,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
         <v>293</v>
       </c>
-      <c r="B15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>383</v>
-      </c>
-      <c r="D15" t="s">
-        <v>293</v>
       </c>
       <c r="E15" t="s">
         <v>200</v>
@@ -2176,16 +2176,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>384</v>
+      </c>
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
         <v>294</v>
       </c>
-      <c r="B16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>384</v>
-      </c>
-      <c r="D16" t="s">
-        <v>294</v>
       </c>
       <c r="E16" t="s">
         <v>201</v>
@@ -2205,16 +2205,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>385</v>
+      </c>
+      <c r="B17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" t="s">
         <v>295</v>
       </c>
-      <c r="B17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>385</v>
-      </c>
-      <c r="D17" t="s">
-        <v>295</v>
       </c>
       <c r="E17" t="s">
         <v>202</v>
@@ -2234,16 +2234,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" t="s">
         <v>296</v>
       </c>
-      <c r="B18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>386</v>
-      </c>
-      <c r="D18" t="s">
-        <v>296</v>
       </c>
       <c r="E18" t="s">
         <v>203</v>
@@ -2263,16 +2263,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
         <v>297</v>
       </c>
-      <c r="B19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>387</v>
-      </c>
-      <c r="D19" t="s">
-        <v>297</v>
       </c>
       <c r="E19" t="s">
         <v>204</v>
@@ -2292,16 +2292,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" t="s">
         <v>298</v>
       </c>
-      <c r="B20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>388</v>
-      </c>
-      <c r="D20" t="s">
-        <v>298</v>
       </c>
       <c r="E20" t="s">
         <v>205</v>
@@ -2321,16 +2321,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>389</v>
+      </c>
+      <c r="B21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" t="s">
         <v>299</v>
       </c>
-      <c r="B21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>389</v>
-      </c>
-      <c r="D21" t="s">
-        <v>299</v>
       </c>
       <c r="E21" t="s">
         <v>206</v>
@@ -2350,16 +2350,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>390</v>
+      </c>
+      <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" t="s">
         <v>300</v>
       </c>
-      <c r="B22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>390</v>
-      </c>
-      <c r="D22" t="s">
-        <v>300</v>
       </c>
       <c r="E22" t="s">
         <v>207</v>
@@ -2379,16 +2379,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>391</v>
+      </c>
+      <c r="B23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" t="s">
         <v>301</v>
       </c>
-      <c r="B23" t="s">
-        <v>186</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>391</v>
-      </c>
-      <c r="D23" t="s">
-        <v>301</v>
       </c>
       <c r="E23" t="s">
         <v>208</v>
@@ -2408,16 +2408,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>392</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
         <v>302</v>
       </c>
-      <c r="B24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>392</v>
-      </c>
-      <c r="D24" t="s">
-        <v>302</v>
       </c>
       <c r="E24" t="s">
         <v>209</v>
@@ -2437,16 +2437,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>393</v>
+      </c>
+      <c r="B25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" t="s">
         <v>303</v>
       </c>
-      <c r="B25" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>393</v>
-      </c>
-      <c r="D25" t="s">
-        <v>303</v>
       </c>
       <c r="E25" t="s">
         <v>210</v>
@@ -2466,16 +2466,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>394</v>
+      </c>
+      <c r="B26" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" t="s">
         <v>304</v>
       </c>
-      <c r="B26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>394</v>
-      </c>
-      <c r="D26" t="s">
-        <v>304</v>
       </c>
       <c r="E26" t="s">
         <v>211</v>
@@ -2495,16 +2495,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>395</v>
+      </c>
+      <c r="B27" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" t="s">
         <v>305</v>
       </c>
-      <c r="B27" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>395</v>
-      </c>
-      <c r="D27" t="s">
-        <v>305</v>
       </c>
       <c r="E27" t="s">
         <v>212</v>
@@ -2524,16 +2524,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>396</v>
+      </c>
+      <c r="B28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" t="s">
         <v>306</v>
       </c>
-      <c r="B28" t="s">
-        <v>186</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>396</v>
-      </c>
-      <c r="D28" t="s">
-        <v>306</v>
       </c>
       <c r="E28" t="s">
         <v>213</v>
@@ -2553,16 +2553,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>397</v>
+      </c>
+      <c r="B29" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" t="s">
         <v>307</v>
       </c>
-      <c r="B29" t="s">
-        <v>186</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>397</v>
-      </c>
-      <c r="D29" t="s">
-        <v>307</v>
       </c>
       <c r="E29" t="s">
         <v>214</v>
@@ -2582,16 +2582,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>398</v>
+      </c>
+      <c r="B30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30" t="s">
         <v>308</v>
       </c>
-      <c r="B30" t="s">
-        <v>186</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>398</v>
-      </c>
-      <c r="D30" t="s">
-        <v>308</v>
       </c>
       <c r="E30" t="s">
         <v>215</v>
@@ -2611,16 +2611,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>399</v>
+      </c>
+      <c r="B31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" t="s">
         <v>309</v>
       </c>
-      <c r="B31" t="s">
-        <v>186</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>399</v>
-      </c>
-      <c r="D31" t="s">
-        <v>309</v>
       </c>
       <c r="E31" t="s">
         <v>216</v>
@@ -2640,16 +2640,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>400</v>
+      </c>
+      <c r="B32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
         <v>310</v>
       </c>
-      <c r="B32" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>400</v>
-      </c>
-      <c r="D32" t="s">
-        <v>310</v>
       </c>
       <c r="E32" t="s">
         <v>217</v>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>401</v>
+      </c>
+      <c r="B33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" t="s">
         <v>311</v>
       </c>
-      <c r="B33" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>401</v>
-      </c>
-      <c r="D33" t="s">
-        <v>311</v>
       </c>
       <c r="E33" t="s">
         <v>218</v>
@@ -2698,16 +2698,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>402</v>
+      </c>
+      <c r="B34" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" t="s">
         <v>312</v>
       </c>
-      <c r="B34" t="s">
-        <v>186</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>402</v>
-      </c>
-      <c r="D34" t="s">
-        <v>312</v>
       </c>
       <c r="E34" t="s">
         <v>219</v>
@@ -2727,16 +2727,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>403</v>
+      </c>
+      <c r="B35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" t="s">
         <v>313</v>
       </c>
-      <c r="B35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>403</v>
-      </c>
-      <c r="D35" t="s">
-        <v>313</v>
       </c>
       <c r="E35" t="s">
         <v>220</v>
@@ -2756,16 +2756,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>404</v>
+      </c>
+      <c r="B36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" t="s">
         <v>314</v>
       </c>
-      <c r="B36" t="s">
-        <v>186</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>404</v>
-      </c>
-      <c r="D36" t="s">
-        <v>314</v>
       </c>
       <c r="E36" t="s">
         <v>221</v>
@@ -2785,16 +2785,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>405</v>
+      </c>
+      <c r="B37" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" t="s">
         <v>315</v>
       </c>
-      <c r="B37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>405</v>
-      </c>
-      <c r="D37" t="s">
-        <v>315</v>
       </c>
       <c r="E37" t="s">
         <v>222</v>
@@ -2814,16 +2814,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>406</v>
+      </c>
+      <c r="B38" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" t="s">
         <v>316</v>
       </c>
-      <c r="B38" t="s">
-        <v>186</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>406</v>
-      </c>
-      <c r="D38" t="s">
-        <v>316</v>
       </c>
       <c r="E38" t="s">
         <v>223</v>
@@ -2843,16 +2843,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>407</v>
+      </c>
+      <c r="B39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" t="s">
         <v>317</v>
       </c>
-      <c r="B39" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>407</v>
-      </c>
-      <c r="D39" t="s">
-        <v>317</v>
       </c>
       <c r="E39" t="s">
         <v>224</v>
@@ -2872,16 +2872,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>408</v>
+      </c>
+      <c r="B40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" t="s">
         <v>318</v>
       </c>
-      <c r="B40" t="s">
-        <v>186</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>408</v>
-      </c>
-      <c r="D40" t="s">
-        <v>318</v>
       </c>
       <c r="E40" t="s">
         <v>225</v>
@@ -2901,16 +2901,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>409</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" t="s">
         <v>319</v>
       </c>
-      <c r="B41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>409</v>
-      </c>
-      <c r="D41" t="s">
-        <v>319</v>
       </c>
       <c r="E41" t="s">
         <v>226</v>
@@ -2930,16 +2930,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>410</v>
+      </c>
+      <c r="B42" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" t="s">
         <v>320</v>
       </c>
-      <c r="B42" t="s">
-        <v>186</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>410</v>
-      </c>
-      <c r="D42" t="s">
-        <v>320</v>
       </c>
       <c r="E42" t="s">
         <v>227</v>
@@ -2959,16 +2959,16 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>411</v>
+      </c>
+      <c r="B43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" t="s">
         <v>321</v>
       </c>
-      <c r="B43" t="s">
-        <v>186</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>411</v>
-      </c>
-      <c r="D43" t="s">
-        <v>321</v>
       </c>
       <c r="E43" t="s">
         <v>228</v>
@@ -2988,16 +2988,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>412</v>
+      </c>
+      <c r="B44" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" t="s">
         <v>322</v>
       </c>
-      <c r="B44" t="s">
-        <v>186</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>412</v>
-      </c>
-      <c r="D44" t="s">
-        <v>322</v>
       </c>
       <c r="E44" t="s">
         <v>229</v>
@@ -3017,16 +3017,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>413</v>
+      </c>
+      <c r="B45" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" t="s">
         <v>323</v>
       </c>
-      <c r="B45" t="s">
-        <v>186</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>413</v>
-      </c>
-      <c r="D45" t="s">
-        <v>323</v>
       </c>
       <c r="E45" t="s">
         <v>230</v>
@@ -3046,16 +3046,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>414</v>
+      </c>
+      <c r="B46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" t="s">
         <v>324</v>
       </c>
-      <c r="B46" t="s">
-        <v>186</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>414</v>
-      </c>
-      <c r="D46" t="s">
-        <v>324</v>
       </c>
       <c r="E46" t="s">
         <v>231</v>
@@ -3075,16 +3075,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>415</v>
+      </c>
+      <c r="B47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" t="s">
         <v>325</v>
       </c>
-      <c r="B47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>415</v>
-      </c>
-      <c r="D47" t="s">
-        <v>325</v>
       </c>
       <c r="E47" t="s">
         <v>232</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>416</v>
+      </c>
+      <c r="B48" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" t="s">
         <v>326</v>
       </c>
-      <c r="B48" t="s">
-        <v>186</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>416</v>
-      </c>
-      <c r="D48" t="s">
-        <v>326</v>
       </c>
       <c r="E48" t="s">
         <v>233</v>
@@ -3133,16 +3133,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>417</v>
+      </c>
+      <c r="B49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" t="s">
         <v>327</v>
       </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>417</v>
-      </c>
-      <c r="D49" t="s">
-        <v>327</v>
       </c>
       <c r="E49" t="s">
         <v>234</v>
@@ -3162,16 +3162,16 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>418</v>
+      </c>
+      <c r="B50" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" t="s">
         <v>328</v>
       </c>
-      <c r="B50" t="s">
-        <v>186</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>418</v>
-      </c>
-      <c r="D50" t="s">
-        <v>328</v>
       </c>
       <c r="E50" t="s">
         <v>235</v>
@@ -3191,16 +3191,16 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>419</v>
+      </c>
+      <c r="B51" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" t="s">
         <v>329</v>
       </c>
-      <c r="B51" t="s">
-        <v>186</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>419</v>
-      </c>
-      <c r="D51" t="s">
-        <v>329</v>
       </c>
       <c r="E51" t="s">
         <v>236</v>
@@ -3220,16 +3220,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>420</v>
+      </c>
+      <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="s">
         <v>330</v>
       </c>
-      <c r="B52" t="s">
-        <v>186</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>420</v>
-      </c>
-      <c r="D52" t="s">
-        <v>330</v>
       </c>
       <c r="E52" t="s">
         <v>237</v>
@@ -3249,16 +3249,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>421</v>
+      </c>
+      <c r="B53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" t="s">
         <v>331</v>
       </c>
-      <c r="B53" t="s">
-        <v>186</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>421</v>
-      </c>
-      <c r="D53" t="s">
-        <v>331</v>
       </c>
       <c r="E53" t="s">
         <v>238</v>
@@ -3278,16 +3278,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>422</v>
+      </c>
+      <c r="B54" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" t="s">
         <v>332</v>
       </c>
-      <c r="B54" t="s">
-        <v>186</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>422</v>
-      </c>
-      <c r="D54" t="s">
-        <v>332</v>
       </c>
       <c r="E54" t="s">
         <v>239</v>
@@ -3307,16 +3307,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>423</v>
+      </c>
+      <c r="B55" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" t="s">
         <v>333</v>
       </c>
-      <c r="B55" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>423</v>
-      </c>
-      <c r="D55" t="s">
-        <v>333</v>
       </c>
       <c r="E55" t="s">
         <v>240</v>
@@ -3336,16 +3336,16 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>424</v>
+      </c>
+      <c r="B56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" t="s">
         <v>334</v>
       </c>
-      <c r="B56" t="s">
-        <v>186</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>424</v>
-      </c>
-      <c r="D56" t="s">
-        <v>334</v>
       </c>
       <c r="E56" t="s">
         <v>241</v>
@@ -3365,16 +3365,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>425</v>
+      </c>
+      <c r="B57" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" t="s">
         <v>335</v>
       </c>
-      <c r="B57" t="s">
-        <v>186</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>425</v>
-      </c>
-      <c r="D57" t="s">
-        <v>335</v>
       </c>
       <c r="E57" t="s">
         <v>242</v>
@@ -3394,16 +3394,16 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>426</v>
+      </c>
+      <c r="B58" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" t="s">
         <v>336</v>
       </c>
-      <c r="B58" t="s">
-        <v>186</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>426</v>
-      </c>
-      <c r="D58" t="s">
-        <v>336</v>
       </c>
       <c r="E58" t="s">
         <v>243</v>
@@ -3423,16 +3423,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>427</v>
+      </c>
+      <c r="B59" t="s">
+        <v>186</v>
+      </c>
+      <c r="C59" t="s">
         <v>337</v>
       </c>
-      <c r="B59" t="s">
-        <v>186</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>427</v>
-      </c>
-      <c r="D59" t="s">
-        <v>337</v>
       </c>
       <c r="E59" t="s">
         <v>244</v>
@@ -3452,16 +3452,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>428</v>
+      </c>
+      <c r="B60" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" t="s">
         <v>338</v>
       </c>
-      <c r="B60" t="s">
-        <v>186</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>428</v>
-      </c>
-      <c r="D60" t="s">
-        <v>338</v>
       </c>
       <c r="E60" t="s">
         <v>245</v>
@@ -3481,16 +3481,16 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>429</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" t="s">
         <v>339</v>
       </c>
-      <c r="B61" t="s">
-        <v>186</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>429</v>
-      </c>
-      <c r="D61" t="s">
-        <v>339</v>
       </c>
       <c r="E61" t="s">
         <v>246</v>
@@ -3510,16 +3510,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>430</v>
+      </c>
+      <c r="B62" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" t="s">
         <v>340</v>
       </c>
-      <c r="B62" t="s">
-        <v>186</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>430</v>
-      </c>
-      <c r="D62" t="s">
-        <v>340</v>
       </c>
       <c r="E62" t="s">
         <v>247</v>
@@ -3539,16 +3539,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>431</v>
+      </c>
+      <c r="B63" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" t="s">
         <v>341</v>
       </c>
-      <c r="B63" t="s">
-        <v>186</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>431</v>
-      </c>
-      <c r="D63" t="s">
-        <v>341</v>
       </c>
       <c r="E63" t="s">
         <v>248</v>
@@ -3568,16 +3568,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>432</v>
+      </c>
+      <c r="B64" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" t="s">
         <v>342</v>
       </c>
-      <c r="B64" t="s">
-        <v>186</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>432</v>
-      </c>
-      <c r="D64" t="s">
-        <v>342</v>
       </c>
       <c r="E64" t="s">
         <v>249</v>
@@ -3597,16 +3597,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>433</v>
+      </c>
+      <c r="B65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" t="s">
         <v>343</v>
       </c>
-      <c r="B65" t="s">
-        <v>186</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>433</v>
-      </c>
-      <c r="D65" t="s">
-        <v>343</v>
       </c>
       <c r="E65" t="s">
         <v>250</v>
@@ -3626,16 +3626,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>434</v>
+      </c>
+      <c r="B66" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" t="s">
         <v>344</v>
       </c>
-      <c r="B66" t="s">
-        <v>186</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>434</v>
-      </c>
-      <c r="D66" t="s">
-        <v>344</v>
       </c>
       <c r="E66" t="s">
         <v>251</v>
@@ -3655,16 +3655,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>435</v>
+      </c>
+      <c r="B67" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" t="s">
         <v>345</v>
       </c>
-      <c r="B67" t="s">
-        <v>186</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>435</v>
-      </c>
-      <c r="D67" t="s">
-        <v>345</v>
       </c>
       <c r="E67" t="s">
         <v>252</v>
@@ -3684,16 +3684,16 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>436</v>
+      </c>
+      <c r="B68" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" t="s">
         <v>346</v>
       </c>
-      <c r="B68" t="s">
-        <v>186</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>436</v>
-      </c>
-      <c r="D68" t="s">
-        <v>346</v>
       </c>
       <c r="E68" t="s">
         <v>253</v>
@@ -3713,16 +3713,16 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>437</v>
+      </c>
+      <c r="B69" t="s">
+        <v>186</v>
+      </c>
+      <c r="C69" t="s">
         <v>347</v>
       </c>
-      <c r="B69" t="s">
-        <v>186</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>437</v>
-      </c>
-      <c r="D69" t="s">
-        <v>347</v>
       </c>
       <c r="E69" t="s">
         <v>254</v>
@@ -3742,16 +3742,16 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>438</v>
+      </c>
+      <c r="B70" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70" t="s">
         <v>348</v>
       </c>
-      <c r="B70" t="s">
-        <v>186</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>438</v>
-      </c>
-      <c r="D70" t="s">
-        <v>348</v>
       </c>
       <c r="E70" t="s">
         <v>255</v>
@@ -3771,16 +3771,16 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>439</v>
+      </c>
+      <c r="B71" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" t="s">
         <v>349</v>
       </c>
-      <c r="B71" t="s">
-        <v>186</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>439</v>
-      </c>
-      <c r="D71" t="s">
-        <v>349</v>
       </c>
       <c r="E71" t="s">
         <v>256</v>
@@ -3800,16 +3800,16 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>440</v>
+      </c>
+      <c r="B72" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" t="s">
         <v>350</v>
       </c>
-      <c r="B72" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>440</v>
-      </c>
-      <c r="D72" t="s">
-        <v>350</v>
       </c>
       <c r="E72" t="s">
         <v>257</v>
@@ -3829,16 +3829,16 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>441</v>
+      </c>
+      <c r="B73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" t="s">
         <v>351</v>
       </c>
-      <c r="B73" t="s">
-        <v>186</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>441</v>
-      </c>
-      <c r="D73" t="s">
-        <v>351</v>
       </c>
       <c r="E73" t="s">
         <v>258</v>
@@ -3858,16 +3858,16 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>442</v>
+      </c>
+      <c r="B74" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" t="s">
         <v>352</v>
       </c>
-      <c r="B74" t="s">
-        <v>186</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>442</v>
-      </c>
-      <c r="D74" t="s">
-        <v>352</v>
       </c>
       <c r="E74" t="s">
         <v>259</v>
@@ -3887,16 +3887,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>443</v>
+      </c>
+      <c r="B75" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" t="s">
         <v>353</v>
       </c>
-      <c r="B75" t="s">
-        <v>186</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>443</v>
-      </c>
-      <c r="D75" t="s">
-        <v>353</v>
       </c>
       <c r="E75" t="s">
         <v>260</v>
@@ -3916,16 +3916,16 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>444</v>
+      </c>
+      <c r="B76" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" t="s">
         <v>354</v>
       </c>
-      <c r="B76" t="s">
-        <v>186</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>444</v>
-      </c>
-      <c r="D76" t="s">
-        <v>354</v>
       </c>
       <c r="E76" t="s">
         <v>261</v>
@@ -3945,16 +3945,16 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>445</v>
+      </c>
+      <c r="B77" t="s">
+        <v>186</v>
+      </c>
+      <c r="C77" t="s">
         <v>355</v>
       </c>
-      <c r="B77" t="s">
-        <v>186</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>445</v>
-      </c>
-      <c r="D77" t="s">
-        <v>355</v>
       </c>
       <c r="E77" t="s">
         <v>262</v>
@@ -3974,16 +3974,16 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>446</v>
+      </c>
+      <c r="B78" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" t="s">
         <v>356</v>
       </c>
-      <c r="B78" t="s">
-        <v>186</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>446</v>
-      </c>
-      <c r="D78" t="s">
-        <v>356</v>
       </c>
       <c r="E78" t="s">
         <v>263</v>
@@ -4003,16 +4003,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>447</v>
+      </c>
+      <c r="B79" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" t="s">
         <v>357</v>
       </c>
-      <c r="B79" t="s">
-        <v>186</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>447</v>
-      </c>
-      <c r="D79" t="s">
-        <v>357</v>
       </c>
       <c r="E79" t="s">
         <v>264</v>
@@ -4032,16 +4032,16 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>448</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" t="s">
         <v>358</v>
       </c>
-      <c r="B80" t="s">
-        <v>186</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>448</v>
-      </c>
-      <c r="D80" t="s">
-        <v>358</v>
       </c>
       <c r="E80" t="s">
         <v>265</v>
@@ -4061,16 +4061,16 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>449</v>
+      </c>
+      <c r="B81" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" t="s">
         <v>359</v>
       </c>
-      <c r="B81" t="s">
-        <v>186</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>449</v>
-      </c>
-      <c r="D81" t="s">
-        <v>359</v>
       </c>
       <c r="E81" t="s">
         <v>266</v>
@@ -4090,16 +4090,16 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>450</v>
+      </c>
+      <c r="B82" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" t="s">
         <v>360</v>
       </c>
-      <c r="B82" t="s">
-        <v>186</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>450</v>
-      </c>
-      <c r="D82" t="s">
-        <v>360</v>
       </c>
       <c r="E82" t="s">
         <v>267</v>
@@ -4119,16 +4119,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>451</v>
+      </c>
+      <c r="B83" t="s">
+        <v>186</v>
+      </c>
+      <c r="C83" t="s">
         <v>361</v>
       </c>
-      <c r="B83" t="s">
-        <v>186</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>451</v>
-      </c>
-      <c r="D83" t="s">
-        <v>361</v>
       </c>
       <c r="E83" t="s">
         <v>268</v>
@@ -4148,16 +4148,16 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>452</v>
+      </c>
+      <c r="B84" t="s">
+        <v>186</v>
+      </c>
+      <c r="C84" t="s">
         <v>362</v>
       </c>
-      <c r="B84" t="s">
-        <v>186</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>452</v>
-      </c>
-      <c r="D84" t="s">
-        <v>362</v>
       </c>
       <c r="E84" t="s">
         <v>269</v>
@@ -4177,16 +4177,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>453</v>
+      </c>
+      <c r="B85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" t="s">
         <v>363</v>
       </c>
-      <c r="B85" t="s">
-        <v>186</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>453</v>
-      </c>
-      <c r="D85" t="s">
-        <v>363</v>
       </c>
       <c r="E85" t="s">
         <v>270</v>
@@ -4206,16 +4206,16 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>454</v>
+      </c>
+      <c r="B86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" t="s">
         <v>364</v>
       </c>
-      <c r="B86" t="s">
-        <v>186</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>454</v>
-      </c>
-      <c r="D86" t="s">
-        <v>364</v>
       </c>
       <c r="E86" t="s">
         <v>271</v>
@@ -4235,16 +4235,16 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>455</v>
+      </c>
+      <c r="B87" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" t="s">
         <v>365</v>
       </c>
-      <c r="B87" t="s">
-        <v>186</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>455</v>
-      </c>
-      <c r="D87" t="s">
-        <v>365</v>
       </c>
       <c r="E87" t="s">
         <v>272</v>
@@ -4264,16 +4264,16 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>456</v>
+      </c>
+      <c r="B88" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" t="s">
         <v>366</v>
       </c>
-      <c r="B88" t="s">
-        <v>186</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>456</v>
-      </c>
-      <c r="D88" t="s">
-        <v>366</v>
       </c>
       <c r="E88" t="s">
         <v>273</v>
@@ -4293,16 +4293,16 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>457</v>
+      </c>
+      <c r="B89" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" t="s">
         <v>367</v>
       </c>
-      <c r="B89" t="s">
-        <v>186</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>457</v>
-      </c>
-      <c r="D89" t="s">
-        <v>367</v>
       </c>
       <c r="E89" t="s">
         <v>274</v>
@@ -4322,16 +4322,16 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>458</v>
+      </c>
+      <c r="B90" t="s">
+        <v>186</v>
+      </c>
+      <c r="C90" t="s">
         <v>368</v>
       </c>
-      <c r="B90" t="s">
-        <v>186</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>458</v>
-      </c>
-      <c r="D90" t="s">
-        <v>368</v>
       </c>
       <c r="E90" t="s">
         <v>275</v>
@@ -4351,16 +4351,16 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>459</v>
+      </c>
+      <c r="B91" t="s">
+        <v>186</v>
+      </c>
+      <c r="C91" t="s">
         <v>369</v>
       </c>
-      <c r="B91" t="s">
-        <v>186</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>459</v>
-      </c>
-      <c r="D91" t="s">
-        <v>369</v>
       </c>
       <c r="E91" t="s">
         <v>276</v>

</xml_diff>